<commit_message>
App upp till buggfix 2 samt uppdat whitebox doc
</commit_message>
<xml_diff>
--- a/Whitebox-testning/whitebox-testning.xlsx
+++ b/Whitebox-testning/whitebox-testning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="29">
   <si>
     <t>Testfall nummer</t>
   </si>
@@ -67,6 +67,42 @@
   </si>
   <si>
     <t>Buggfix 1 - korrigering av funktioner ovan - (uniqueSides()==3) resp 1</t>
+  </si>
+  <si>
+    <t>Unittest isIsoscelesTest() med En sida = 0</t>
+  </si>
+  <si>
+    <t>Unittest isScaleneTest()) med En sida = 0</t>
+  </si>
+  <si>
+    <t>Unittest isEquilateralTest() med En sida = 0</t>
+  </si>
+  <si>
+    <t>1.2, 0, 1.2</t>
+  </si>
+  <si>
+    <t>1.2, 0, 1.3</t>
+  </si>
+  <si>
+    <t>0, 0, 0</t>
+  </si>
+  <si>
+    <t>Triangel kan ej ha en sida = 0</t>
+  </si>
+  <si>
+    <t>Buggfix 2 - kontroll av inparametern i konstruktorn &lt;= 0</t>
+  </si>
+  <si>
+    <t>if ((a &lt;= 0) || (b &lt;= 0) || (c &lt;= 0))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          throw new ArgumentOutOfRangeException("Cannot use a value less or equal to 0 as a side in a triangle");</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      }</t>
   </si>
 </sst>
 </file>
@@ -423,16 +459,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F11"/>
+  <dimension ref="A2:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="101.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1"/>
@@ -522,7 +558,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -539,7 +575,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -556,7 +592,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
@@ -569,6 +605,142 @@
       </c>
       <c r="E11" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
uppdat whitebox doc med test7, ny clean solution
</commit_message>
<xml_diff>
--- a/Whitebox-testning/whitebox-testning.xlsx
+++ b/Whitebox-testning/whitebox-testning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="32">
   <si>
     <t>Testfall nummer</t>
   </si>
@@ -103,6 +103,15 @@
   </si>
   <si>
     <t xml:space="preserve">      }</t>
+  </si>
+  <si>
+    <t>Unittest isScaleneTest()) där en sida större än summan av de två andra</t>
+  </si>
+  <si>
+    <t>1.2, 20, 1.3</t>
+  </si>
+  <si>
+    <t>Buggfix 3 - kontroll av inparametrar i konstruktorn (a + b &lt;= c) || (a + c &lt;= b) || (b + c &lt;= a)</t>
   </si>
 </sst>
 </file>
@@ -459,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F25"/>
+  <dimension ref="A2:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,6 +749,45 @@
         <v>11</v>
       </c>
       <c r="E25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>7</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>7</v>
+      </c>
+      <c r="B32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>